<commit_message>
link analysis - 112919
</commit_message>
<xml_diff>
--- a/aws-cda/aws-link-analysis.xlsx
+++ b/aws-cda/aws-link-analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20700" windowHeight="11760" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20700" windowHeight="11760" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" state="hidden" r:id="rId1"/>
@@ -15895,7 +15895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
@@ -16715,8 +16715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17968,7 +17968,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html" target="_blank"&gt;amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>345</v>
       </c>
@@ -17983,7 +17983,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html" target="_blank"&gt;amazondynamodb/latest/developerguide/Limits&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;5&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>345</v>
       </c>
@@ -17998,7 +17998,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html#limits-capacity-units-provisioned-throughput" target="_blank"&gt;amazondynamodb/latest/developerguide/Limits.html#limits-capacity-units-provisioned-throughput&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>345</v>
       </c>
@@ -18013,7 +18013,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/SecondaryIndexes.html" target="_blank"&gt;amazondynamodb/latest/developerguide/SecondaryIndexes&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>345</v>
       </c>
@@ -18028,7 +18028,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/WorkingWithItems.html" target="_blank"&gt;amazondynamodb/latest/developerguide/WorkingWithItems&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>345</v>
       </c>
@@ -18043,7 +18043,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/WorkingWithTables.html" target="_blank"&gt;amazondynamodb/latest/developerguide/WorkingWithTables&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>345</v>
       </c>
@@ -18058,7 +18058,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/blogs/database/choosing-the-right-dynamodb-partition-key/" target="_blank"&gt;blogs/database/choosing-the-right-dynamodb-partition-key/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>345</v>
       </c>
@@ -18073,7 +18073,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/blogs/developer/elasticache-as-an-asp-net-session-store/ " target="_blank"&gt;blogs/developer/elasticache-as-an-asp-net-session-store/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>345</v>
       </c>
@@ -18088,7 +18088,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/blogs/developer/rate-limited-scans-in-amazon-dynamodb/" target="_blank"&gt;blogs/developer/rate-limited-scans-in-amazon-dynamodb/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>345</v>
       </c>
@@ -18103,7 +18103,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/dynamodb/" target="_blank"&gt;dynamodb/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>345</v>
       </c>
@@ -18118,7 +18118,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/dynamodb/dax/" target="_blank"&gt;dynamodb/dax/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>345</v>
       </c>
@@ -18133,7 +18133,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/dynamodb/faqs/" target="_blank"&gt;dynamodb/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;6&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>345</v>
       </c>
@@ -18148,7 +18148,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/dynamodb/pricing/" target="_blank"&gt;dynamodb/pricing/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>345</v>
       </c>
@@ -18163,7 +18163,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/best-practices.html" target="_blank"&gt;amazondynamodb/latest/developerguide/best-practices&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>345</v>
       </c>
@@ -18178,7 +18178,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/bp-indexes-general.html" target="_blank"&gt;amazondynamodb/latest/developerguide/bp-indexes-general&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>345</v>
       </c>
@@ -18193,7 +18193,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/bp-partition-key-uniform-load.html" target="_blank"&gt;amazondynamodb/latest/developerguide/bp-partition-key-uniform-load&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>345</v>
       </c>
@@ -18208,7 +18208,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/bp-query-scan.html" target="_blank"&gt;amazondynamodb/latest/developerguide/bp-query-scan&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>345</v>
       </c>
@@ -18223,7 +18223,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/DAX.html" target="_blank"&gt;amazondynamodb/latest/developerguide/DAX&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>345</v>
       </c>
@@ -18238,7 +18238,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Expressions.ProjectionExpressions.html" target="_blank"&gt;amazondynamodb/latest/developerguide/Expressions.ProjectionExpressions&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>345</v>
       </c>
@@ -18253,7 +18253,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.API.html" target="_blank"&gt;amazondynamodb/latest/developerguide/HowItWorks.API&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>345</v>
       </c>
@@ -18268,7 +18268,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html" target="_blank"&gt;amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;7&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>345</v>
       </c>
@@ -18283,7 +18283,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ReadWriteCapacityMode.html" target="_blank"&gt;amazondynamodb/latest/developerguide/HowItWorks.ReadWriteCapacityMode&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>345</v>
       </c>
@@ -18298,7 +18298,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html#limits-secondary-indexes" target="_blank"&gt;amazondynamodb/latest/developerguide/Limits.html#limits-secondary-indexes&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>345</v>
       </c>
@@ -18313,7 +18313,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Programming.Errors.html" target="_blank"&gt;amazondynamodb/latest/developerguide/Programming.Errors&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>345</v>
       </c>
@@ -18328,7 +18328,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Query.html" target="_blank"&gt;amazondynamodb/latest/developerguide/Query&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>345</v>
       </c>
@@ -18343,7 +18343,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Query.html" target="_blank"&gt;amazondynamodb/latest/developerguide/Query&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>345</v>
       </c>
@@ -18358,7 +18358,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/SecondaryIndexes.html" target="_blank"&gt;amazondynamodb/latest/developerguide/SecondaryIndexes&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>345</v>
       </c>
@@ -18373,7 +18373,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/specifying-conditions.html" target="_blank"&gt;amazondynamodb/latest/developerguide/specifying-conditions&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>392</v>
       </c>
@@ -18388,7 +18388,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_BundleInstance.html" target="_blank"&gt;AWSEC2/latest/APIReference/API_BundleInstance&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>392</v>
       </c>
@@ -18403,7 +18403,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_DescribeImages.html" target="_blank"&gt;AWSEC2/latest/APIReference/API_DescribeImages&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>392</v>
       </c>
@@ -18418,7 +18418,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/AmazonEBS.html" target="_blank"&gt;AWSEC2/latest/UserGuide/AmazonEBS&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>392</v>
       </c>
@@ -18433,7 +18433,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html" target="_blank"&gt;AWSEC2/latest/UserGuide/ComponentsAMIs&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>392</v>
       </c>
@@ -18448,7 +18448,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSEncryption.html" target="_blank"&gt;AWSEC2/latest/UserGuide/EBSEncryption&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;5&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>392</v>
       </c>
@@ -18463,7 +18463,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSEncryption.html#EBSEncryption_supported_instances" target="_blank"&gt;AWSEC2/latest/UserGuide/EBSEncryption.html#EBSEncryption_supported_instances&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>392</v>
       </c>
@@ -18478,7 +18478,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSSnapshots.html" target="_blank"&gt;AWSEC2/latest/UserGuide/EBSSnapshots&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>392</v>
       </c>
@@ -18493,7 +18493,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSVolumes.html#EBSFeatures" target="_blank"&gt;AWSEC2/latest/UserGuide/EBSVolumes.html#EBSFeatures&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>392</v>
       </c>
@@ -18508,7 +18508,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ec2-instance-metadata.html" target="_blank"&gt;AWSEC2/latest/UserGuide/ec2-instance-metadata&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>392</v>
       </c>
@@ -18523,7 +18523,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/sharingamis-explicit.html" target="_blank"&gt;AWSEC2/latest/UserGuide/sharingamis-explicit&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>392</v>
       </c>
@@ -18538,7 +18538,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/Stop_Start.html" target="_blank"&gt;AWSEC2/latest/UserGuide/Stop_Start&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>392</v>
       </c>
@@ -18553,7 +18553,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/TroubleshootingInstancesConnecting.html#d0e132832" target="_blank"&gt;AWSEC2/latest/UserGuide/TroubleshootingInstancesConnecting.html#d0e132832&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>392</v>
       </c>
@@ -18568,7 +18568,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/using-regions-availability-zones.html" target="_blank"&gt;AWSEC2/latest/UserGuide/using-regions-availability-zones&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>392</v>
       </c>
@@ -18583,7 +18583,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/articles/1233/" target="_blank"&gt;articles/1233/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>392</v>
       </c>
@@ -18598,7 +18598,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/" target="_blank"&gt;blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>392</v>
       </c>
@@ -18613,7 +18613,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/ec2/" target="_blank"&gt;ec2/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>392</v>
       </c>
@@ -18628,7 +18628,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/ec2/faqs/#Billing" target="_blank"&gt;ec2/faqs/#Billing&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>392</v>
       </c>
@@ -18643,7 +18643,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSEC2/latest/UserGuide/CopyingAMIs.html" target="_blank"&gt;AWSEC2/latest/UserGuide/CopyingAMIs&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>392</v>
       </c>
@@ -18658,7 +18658,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSEncryption.html" target="_blank"&gt;AWSEC2/latest/UserGuide/EBSEncryption&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>392</v>
       </c>
@@ -18673,7 +18673,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSEC2/latest/UserGuide/iam-roles-for-amazon-ec2.html" target="_blank"&gt;AWSEC2/latest/UserGuide/iam-roles-for-amazon-ec2&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>392</v>
       </c>
@@ -18688,7 +18688,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSEC2/latest/UserGuide/iam-roles-for-amazon-ec2.html" target="_blank"&gt;AWSEC2/latest/UserGuide/iam-roles-for-amazon-ec2&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>392</v>
       </c>
@@ -18703,7 +18703,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSEC2/latest/UserGuide/user-data.html" target="_blank"&gt;AWSEC2/latest/UserGuide/user-data&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>351</v>
       </c>
@@ -18718,7 +18718,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/ecs/faqs" target="_blank"&gt;ecs/faqs&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>351</v>
       </c>
@@ -18733,7 +18733,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/ecs/faqs/" target="_blank"&gt;ecs/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>351</v>
       </c>
@@ -18748,7 +18748,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/ecs/s3/faqs/" target="_blank"&gt;s3/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>351</v>
       </c>
@@ -18763,7 +18763,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/ecs/sqs/faqs/" target="_blank"&gt;sqs/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>351</v>
       </c>
@@ -18778,8 +18778,8 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/ecs/vpc/faqs/" target="_blank"&gt;vpc/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
         <v>351</v>
       </c>
       <c r="B138" s="6" t="s">
@@ -18793,7 +18793,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonECS/latest/developerguide/task-iam-roles.html" target="_blank"&gt;AmazonECS/latest/developerguide/task-iam-roles&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>352</v>
       </c>
@@ -18808,7 +18808,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/caching/" target="_blank"&gt;caching/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>352</v>
       </c>
@@ -18823,7 +18823,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/elasticache/" target="_blank"&gt;elasticache/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>352</v>
       </c>
@@ -18838,7 +18838,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonElastiCache/latest/mem-ug/Strategies.html" target="_blank"&gt;AmazonElastiCache/latest/mem-ug/Strategies&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>352</v>
       </c>
@@ -18853,7 +18853,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonElastiCache/latest/red-ug/elasticache-use-cases.html" target="_blank"&gt;AmazonElastiCache/latest/red-ug/elasticache-use-cases&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>336</v>
       </c>
@@ -18868,7 +18868,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.CNAMESwap.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.CNAMESwap&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>336</v>
       </c>
@@ -18883,7 +18883,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.environments.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.environments&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>336</v>
       </c>
@@ -18898,7 +18898,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features-managing-env-tiers.html#worker-daemon" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features-managing-env-tiers.html#worker-daemon&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>336</v>
       </c>
@@ -18913,7 +18913,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features-managing-env-tiers.html#worker-deadletter" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features-managing-env-tiers.html#worker-deadletter&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>336</v>
       </c>
@@ -18928,7 +18928,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticbeanstalk/latest/dg/Welcome.html" target="_blank"&gt;elasticbeanstalk/latest/dg/Welcome&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>336</v>
       </c>
@@ -18943,7 +18943,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/elasticbeanstalk/faqs/" target="_blank"&gt;elasticbeanstalk/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>336</v>
       </c>
@@ -18958,7 +18958,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/elasticbeanstalk/faqs/" target="_blank"&gt;elasticbeanstalk/faqs/&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>336</v>
       </c>
@@ -18973,7 +18973,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/applications-sourcebundle.html" target="_blank"&gt;elasticbeanstalk/latest/dg/applications-sourcebundle&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>336</v>
       </c>
@@ -18988,7 +18988,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/applications-sourcebundle.html" target="_blank"&gt;elasticbeanstalk/latest/dg/applications-sourcebundle&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>336</v>
       </c>
@@ -19003,7 +19003,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/applications-versions.html" target="_blank"&gt;elasticbeanstalk/latest/dg/applications-versions&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>336</v>
       </c>
@@ -19018,7 +19018,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/concepts.concepts.design.html" target="_blank"&gt;elasticbeanstalk/latest/dg/concepts.concepts.design&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>336</v>
       </c>
@@ -19033,7 +19033,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/create_deploy_docker.html" target="_blank"&gt;elasticbeanstalk/latest/dg/create_deploy_docker&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>336</v>
       </c>
@@ -19048,7 +19048,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/custom-platforms.html" target="_blank"&gt;elasticbeanstalk/latest/dg/custom-platforms&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>336</v>
       </c>
@@ -19063,7 +19063,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/eb-cli3.html" target="_blank"&gt;elasticbeanstalk/latest/dg/eb-cli3&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>336</v>
       </c>
@@ -19078,7 +19078,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/environment-configuration-methods-before.html" target="_blank"&gt;elasticbeanstalk/latest/dg/environment-configuration-methods-before&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>336</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/environmentmgmt-updates-immutable.html" target="_blank"&gt;elasticbeanstalk/latest/dg/environmentmgmt-updates-immutable&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>336</v>
       </c>
@@ -19108,7 +19108,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/environments-updating.html" target="_blank"&gt;elasticbeanstalk/latest/dg/environments-updating&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>336</v>
       </c>
@@ -19123,7 +19123,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.CNAMESwap.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.CNAMESwap&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>336</v>
       </c>
@@ -19138,7 +19138,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.deploy-existing-version.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.deploy-existing-version&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>336</v>
       </c>
@@ -19153,7 +19153,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.as.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.managing.as&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>336</v>
       </c>
@@ -19168,7 +19168,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.db.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.managing.db&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>336</v>
       </c>
@@ -19183,7 +19183,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.ec2.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.managing.ec2&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>336</v>
       </c>
@@ -19198,7 +19198,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.platform.upgrade.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.platform.upgrade&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>336</v>
       </c>
@@ -19213,7 +19213,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.rolling-version-deploy.html" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.rolling-version-deploy&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>336</v>
       </c>
@@ -19228,7 +19228,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.rolling-version-deploy.html#environments-cfg-rollingdeployments-method" target="_blank"&gt;elasticbeanstalk/latest/dg/using-features.rolling-version-deploy.html#environments-cfg-rollingdeployments-method&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>325</v>
       </c>
@@ -19243,7 +19243,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://aws.amazon.com/articles/1636185810492479" target="_blank"&gt;http://aws.amazon.com/articles/1636185810492479&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>325</v>
       </c>
@@ -19258,7 +19258,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticloadbalancing/latest/classic/elb-getting-started.html" target="_blank"&gt;elasticloadbalancing/latest/classic/elb-getting-started&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>325</v>
       </c>
@@ -19273,7 +19273,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticloadbalancing/latest/classic/elb-security-groups.html#elb-classic-security-groups" target="_blank"&gt;elasticloadbalancing/latest/classic/elb-security-groups.html#elb-classic-security-groups&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>325</v>
       </c>
@@ -19288,7 +19288,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/elasticloadbalancing/latest/userguide/how-elastic-load-balancing-works.html" target="_blank"&gt;elasticloadbalancing/latest/userguide/how-elastic-load-balancing-works&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>325</v>
       </c>
@@ -19303,7 +19303,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/articles/1636185810492479" target="_blank"&gt;articles/1636185810492479&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>325</v>
       </c>
@@ -19318,7 +19318,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticloadbalancing/latest/application/load-balancer-access-logs.html" target="_blank"&gt;elasticloadbalancing/latest/application/load-balancer-access-logs&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>325</v>
       </c>
@@ -19333,7 +19333,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/elasticloadbalancing/latest/application/load-balancer-troubleshooting.html" target="_blank"&gt;elasticloadbalancing/latest/application/load-balancer-troubleshooting&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>371</v>
       </c>
@@ -19348,7 +19348,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/firehose/latest/dev/encryption.html" target="_blank"&gt;firehose/latest/dev/encryption&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>337</v>
       </c>
@@ -19363,7 +19363,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/general/latest/gr/aws_service_limits.html" target="_blank"&gt;general/latest/gr/aws_service_limits&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>337</v>
       </c>
@@ -19378,7 +19378,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sdk-for-javascript/v2/developer-guide/config-web-identity-examples.html" target="_blank"&gt;sdk-for-javascript/v2/developer-guide/config-web-identity-examples&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>337</v>
       </c>
@@ -19393,7 +19393,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/tools/" target="_blank"&gt;tools/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>337</v>
       </c>
@@ -19408,7 +19408,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/aws-technical-content/latest/microservices-on-aws/simple-microservices-architecture-on-aws.html" target="_blank"&gt;aws-technical-content/latest/microservices-on-aws/simple-microservices-architecture-on-aws&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>337</v>
       </c>
@@ -19423,7 +19423,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/general/latest/gr/api-retries.html" target="_blank"&gt;general/latest/gr/api-retries&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>337</v>
       </c>
@@ -19438,7 +19438,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/general/latest/gr/api-retries.html" target="_blank"&gt;general/latest/gr/api-retries&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>337</v>
       </c>
@@ -19453,7 +19453,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/general/latest/gr/aws-sec-cred-types.html" target="_blank"&gt;general/latest/gr/aws-sec-cred-types&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;6&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>337</v>
       </c>
@@ -19468,7 +19468,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/general/latest/gr/signing_aws_api_requests.html" target="_blank"&gt;general/latest/gr/signing_aws_api_requests&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>337</v>
       </c>
@@ -19483,7 +19483,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://forums.aws.amazon.com/thread.jspa?messageID=604424" target="_blank"&gt;thread.jspa?messageID=604424&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>359</v>
       </c>
@@ -19498,7 +19498,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/id_credentials_mfa.html" target="_blank"&gt;IAM/latest/UserGuide/id_credentials_mfa&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>359</v>
       </c>
@@ -19513,7 +19513,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/id_roles.html" target="_blank"&gt;IAM/latest/UserGuide/id_roles&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>359</v>
       </c>
@@ -19528,7 +19528,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/id_roles_providers.html" target="_blank"&gt;IAM/latest/UserGuide/id_roles_providers&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>359</v>
       </c>
@@ -19543,7 +19543,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/id_roles_providers.html" target="_blank"&gt;IAM/latest/UserGuide/id_roles_providers&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>359</v>
       </c>
@@ -19558,7 +19558,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/id_roles_providers_oidc.html" target="_blank"&gt;IAM/latest/UserGuide/id_roles_providers_oidc&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>359</v>
       </c>
@@ -19573,7 +19573,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/reference_iam-limits.html" target="_blank"&gt;IAM/latest/UserGuide/reference_iam-limits&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>359</v>
       </c>
@@ -19588,7 +19588,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/reference_policies_evaluation-logic.html" target="_blank"&gt;IAM/latest/UserGuide/reference_policies_evaluation-logic&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>359</v>
       </c>
@@ -19603,7 +19603,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://console.aws.amazon.com/iam/" target="_blank"&gt;https://console.aws.amazon.com/iam/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>359</v>
       </c>
@@ -19618,7 +19618,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://console.aws.amazon.com/support/home#/case/create?issueType=service-limit-increase&amp;limitType=service-code-iam-groups-and-users" target="_blank"&gt;https://console.aws.amazon.com/support/home#/case/create?issueType=service-limit-increase&amp;limitType=service-code-iam-groups-and-users&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>359</v>
       </c>
@@ -19633,7 +19633,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/access_policies_testing-policies.html" target="_blank"&gt;IAM/latest/UserGuide/access_policies_testing-policies&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>359</v>
       </c>
@@ -19648,7 +19648,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/cloudtrail-integration.html" target="_blank"&gt;IAM/latest/UserGuide/cloudtrail-integration&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>359</v>
       </c>
@@ -19663,7 +19663,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/id_credentials_temp_request.html" target="_blank"&gt;IAM/latest/UserGuide/id_credentials_temp_request&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>359</v>
       </c>
@@ -19678,7 +19678,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/id_roles_create_for-user_externalid.html" target="_blank"&gt;IAM/latest/UserGuide/id_roles_create_for-user_externalid&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>359</v>
       </c>
@@ -19693,7 +19693,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/id_roles_providers_oidc.html" target="_blank"&gt;IAM/latest/UserGuide/id_roles_providers_oidc&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>359</v>
       </c>
@@ -19708,7 +19708,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/id_roles_use_switch-role-api.html" target="_blank"&gt;IAM/latest/UserGuide/id_roles_use_switch-role-api&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>359</v>
       </c>
@@ -19723,7 +19723,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/reference_policies_variables.html" target="_blank"&gt;IAM/latest/UserGuide/reference_policies_variables&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>359</v>
       </c>
@@ -19738,7 +19738,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/IAM/latest/UserGuide/tutorial_cross-account-with-roles.html" target="_blank"&gt;IAM/latest/UserGuide/tutorial_cross-account-with-roles&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>346</v>
       </c>
@@ -19753,7 +19753,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/" target="_blank"&gt;blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>346</v>
       </c>
@@ -19768,7 +19768,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/kinesis/" target="_blank"&gt;kinesis/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>340</v>
       </c>
@@ -19783,7 +19783,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/kms/latest/developerguide/services-ebs.html#ebs-encrypt" target="_blank"&gt;kms/latest/developerguide/services-ebs.html#ebs-encrypt&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>340</v>
       </c>
@@ -19798,7 +19798,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/kms/latest/APIReference/API_GenerateDataKey.html" target="_blank"&gt;kms/latest/APIReference/API_GenerateDataKey&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>340</v>
       </c>
@@ -19813,7 +19813,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/kms/latest/APIReference/API_GenerateDataKeyWithoutPlaintext.html" target="_blank"&gt;kms/latest/APIReference/API_GenerateDataKeyWithoutPlaintext&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>341</v>
       </c>
@@ -19828,7 +19828,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/lambda/latest/dg/limits.html" target="_blank"&gt;lambda/latest/dg/limits&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>341</v>
       </c>
@@ -19843,7 +19843,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/en_pv/lambda/latest/dg/invocation-async.html" target="_blank"&gt;en_pv/lambda/latest/dg/invocation-async&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>341</v>
       </c>
@@ -19858,7 +19858,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/automating-deployment.html" target="_blank"&gt;lambda/latest/dg/automating-deployment&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>341</v>
       </c>
@@ -19873,7 +19873,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/best-practices.html" target="_blank"&gt;lambda/latest/dg/best-practices&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>341</v>
       </c>
@@ -19888,7 +19888,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/best-practices.html" target="_blank"&gt;lambda/latest/dg/best-practices&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>341</v>
       </c>
@@ -19903,7 +19903,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/best-practices.html#function-code" target="_blank"&gt;lambda/latest/dg/best-practices.html#function-code&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>341</v>
       </c>
@@ -19918,7 +19918,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/current-supported-versions.html" target="_blank"&gt;lambda/latest/dg/current-supported-versions&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>341</v>
       </c>
@@ -19933,7 +19933,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/enabling-x-ray.html" target="_blank"&gt;lambda/latest/dg/enabling-x-ray&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>341</v>
       </c>
@@ -19948,7 +19948,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/env_variables.html" target="_blank"&gt;lambda/latest/dg/env_variables&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>341</v>
       </c>
@@ -19963,7 +19963,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/get-started-create-function.html" target="_blank"&gt;lambda/latest/dg/get-started-create-function&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>341</v>
       </c>
@@ -19978,7 +19978,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/invoking-lambda-function.html" target="_blank"&gt;lambda/latest/dg/invoking-lambda-function&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>341</v>
       </c>
@@ -19993,7 +19993,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/lambda-traffic-shifting-using-aliases.html" target="_blank"&gt;lambda/latest/dg/lambda-traffic-shifting-using-aliases&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>341</v>
       </c>
@@ -20008,7 +20008,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/lambda-x-ray.html" target="_blank"&gt;lambda/latest/dg/lambda-x-ray&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>341</v>
       </c>
@@ -20023,7 +20023,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/lcome.html" target="_blank"&gt;lambda/latest/dg/lcome&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>341</v>
       </c>
@@ -20038,7 +20038,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/limits.html" target="_blank"&gt;lambda/latest/dg/limits&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;5&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>341</v>
       </c>
@@ -20053,7 +20053,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/monitoring-functions.html" target="_blank"&gt;lambda/latest/dg/monitoring-functions&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>341</v>
       </c>
@@ -20068,7 +20068,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/monitoring-functions-access-metrics.html" target="_blank"&gt;lambda/latest/dg/monitoring-functions-access-metrics&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>341</v>
       </c>
@@ -20083,7 +20083,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/serverless-deploy-wt.html" target="_blank"&gt;lambda/latest/dg/serverless-deploy-wt&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>341</v>
       </c>
@@ -20098,7 +20098,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/troubleshooting.html" target="_blank"&gt;lambda/latest/dg/troubleshooting&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>341</v>
       </c>
@@ -20113,7 +20113,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/vpc.html" target="_blank"&gt;lambda/latest/dg/vpc&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>341</v>
       </c>
@@ -20128,7 +20128,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/with-ddb.html" target="_blank"&gt;lambda/latest/dg/with-ddb&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>341</v>
       </c>
@@ -20143,7 +20143,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/with-s3.html" target="_blank"&gt;lambda/latest/dg/with-s3&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>341</v>
       </c>
@@ -20158,7 +20158,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/with-sqs.html" target="_blank"&gt;lambda/latest/dg/with-sqs&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>341</v>
       </c>
@@ -20173,7 +20173,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/lambda/latest/dg/with-userapp-walkthrough-custom-events-create-iam-role.html" target="_blank"&gt;lambda/latest/dg/with-userapp-walkthrough-custom-events-create-iam-role&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>373</v>
       </c>
@@ -20188,7 +20188,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/opsworks/latest/userguide/troubleshoot-debug.html" target="_blank"&gt;opsworks/latest/userguide/troubleshoot-debug&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>357</v>
       </c>
@@ -20203,7 +20203,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonRDS/latest/UserGuide/Concepts.MultiAZ.html" target="_blank"&gt;AmazonRDS/latest/UserGuide/Concepts.MultiAZ&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>357</v>
       </c>
@@ -20218,7 +20218,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonRDS/latest/UserGuide/Concepts.MultiAZ.html#Concepts.MultiAZ.Failover" target="_blank"&gt;AmazonRDS/latest/UserGuide/Concepts.MultiAZ.html#Concepts.MultiAZ.Failover&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>357</v>
       </c>
@@ -20233,7 +20233,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonRDS/latest/UserGuide/USER_PIT.html" target="_blank"&gt;AmazonRDS/latest/UserGuide/USER_PIT&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>357</v>
       </c>
@@ -20248,7 +20248,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/rds/details/read-replicas/" target="_blank"&gt;rds/details/read-replicas/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>357</v>
       </c>
@@ -20263,7 +20263,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/rds/faqs/" target="_blank"&gt;rds/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>357</v>
       </c>
@@ -20278,7 +20278,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonRDS/latest/UserGuide/USER_ConnectToInstance.html" target="_blank"&gt;AmazonRDS/latest/UserGuide/USER_ConnectToInstance&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>357</v>
       </c>
@@ -20293,7 +20293,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonRDS/latest/UserGuide/UsingWithRDS.SSL.html" target="_blank"&gt;AmazonRDS/latest/UserGuide/UsingWithRDS.SSL&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>372</v>
       </c>
@@ -20308,7 +20308,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/redshift/latest/gsg/rs-gsg-create-sample-db.html" target="_blank"&gt;redshift/latest/gsg/rs-gsg-create-sample-db&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>375</v>
       </c>
@@ -20323,7 +20323,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/Route53/latest/DeveloperGuide/dns-failover.html" target="_blank"&gt;Route53/latest/DeveloperGuide/dns-failover&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>375</v>
       </c>
@@ -20338,7 +20338,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/Route53/latest/DeveloperGuide/routing-policy.html#routing-policy-weighted" target="_blank"&gt;Route53/latest/DeveloperGuide/routing-policy.html#routing-policy-weighted&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>350</v>
       </c>
@@ -20353,7 +20353,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/API/ErrorResponses.html" target="_blank"&gt;AmazonS3/latest/API/ErrorResponses&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>350</v>
       </c>
@@ -20368,7 +20368,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/API/RESTObjectGET.html" target="_blank"&gt;AmazonS3/latest/API/RESTObjectGET&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>350</v>
       </c>
@@ -20383,7 +20383,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/access-policy-language-overview.html" target="_blank"&gt;AmazonS3/latest/dev/access-policy-language-overview&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>350</v>
       </c>
@@ -20398,7 +20398,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/acl-overview.html#canned-acl" target="_blank"&gt;AmazonS3/latest/dev/acl-overview.html#canned-acl&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>350</v>
       </c>
@@ -20413,7 +20413,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/example-bucket-policies.html#example-bucket-policies-use-case-3" target="_blank"&gt;AmazonS3/latest/dev/example-bucket-policies.html#example-bucket-policies-use-case-3&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>350</v>
       </c>
@@ -20428,7 +20428,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/mpuoverview.html" target="_blank"&gt;AmazonS3/latest/dev/mpuoverview&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>350</v>
       </c>
@@ -20443,7 +20443,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/NotificationHowTo.html" target="_blank"&gt;AmazonS3/latest/dev/NotificationHowTo&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>350</v>
       </c>
@@ -20458,7 +20458,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/ObjectVersioning.html" target="_blank"&gt;AmazonS3/latest/dev/ObjectVersioning&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>350</v>
       </c>
@@ -20473,7 +20473,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/request-rate-perf-considerations.html" target="_blank"&gt;AmazonS3/latest/dev/request-rate-perf-considerations&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>350</v>
       </c>
@@ -20488,7 +20488,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/s3-access-control.html" target="_blank"&gt;AmazonS3/latest/dev/s3-access-control&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>350</v>
       </c>
@@ -20503,7 +20503,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/ServerLogs.html" target="_blank"&gt;AmazonS3/latest/dev/ServerLogs&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>350</v>
       </c>
@@ -20518,7 +20518,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/ServerSideEncryptionCustomerKeys.html" target="_blank"&gt;AmazonS3/latest/dev/ServerSideEncryptionCustomerKeys&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>350</v>
       </c>
@@ -20533,7 +20533,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/serv-side-encryption.html" target="_blank"&gt;AmazonS3/latest/dev/serv-side-encryption&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>350</v>
       </c>
@@ -20548,7 +20548,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/UsingClientSideEncryption.html" target="_blank"&gt;AmazonS3/latest/dev/UsingClientSideEncryption&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>350</v>
       </c>
@@ -20563,7 +20563,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/UsingEncryption.html" target="_blank"&gt;AmazonS3/latest/dev/UsingEncryption&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>350</v>
       </c>
@@ -20578,7 +20578,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/WebsiteHosting.html" target="_blank"&gt;AmazonS3/latest/dev/WebsiteHosting&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>350</v>
       </c>
@@ -20593,7 +20593,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/" target="_blank"&gt;about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>350</v>
       </c>
@@ -20608,7 +20608,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/premiumsupport/knowledge-center/s3-bucket-performance-improve/" target="_blank"&gt;premiumsupport/knowledge-center/s3-bucket-performance-improve/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>350</v>
       </c>
@@ -20623,7 +20623,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/s3/faqs/" target="_blank"&gt;s3/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>350</v>
       </c>
@@ -20638,7 +20638,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/API/ErrorResponses.html" target="_blank"&gt;AmazonS3/latest/API/ErrorResponses&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>350</v>
       </c>
@@ -20653,7 +20653,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/API/ErrorResponses.html#ErrorCodeList" target="_blank"&gt;AmazonS3/latest/API/ErrorResponses.html#ErrorCodeList&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>350</v>
       </c>
@@ -20668,7 +20668,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/API/RESTObjectOps.html" target="_blank"&gt;AmazonS3/latest/API/RESTObjectOps&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>350</v>
       </c>
@@ -20683,7 +20683,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/access-policy-language-overview.html" target="_blank"&gt;AmazonS3/latest/dev/access-policy-language-overview&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>350</v>
       </c>
@@ -20698,7 +20698,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/cors.html" target="_blank"&gt;AmazonS3/latest/dev/cors&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>350</v>
       </c>
@@ -20713,7 +20713,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/optimizing-performance.html" target="_blank"&gt;AmazonS3/latest/dev/optimizing-performance&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>350</v>
       </c>
@@ -20728,7 +20728,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/request-rate-perf-considerations.html" target="_blank"&gt;AmazonS3/latest/dev/request-rate-perf-considerations&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;4&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>350</v>
       </c>
@@ -20743,7 +20743,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/ServerSideEncryptionCustomerKeys.html" target="_blank"&gt;AmazonS3/latest/dev/ServerSideEncryptionCustomerKeys&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>350</v>
       </c>
@@ -20758,7 +20758,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/serv-side-encryption.html" target="_blank"&gt;AmazonS3/latest/dev/serv-side-encryption&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>350</v>
       </c>
@@ -20773,7 +20773,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/SSEUsingRESTAPI.html" target="_blank"&gt;AmazonS3/latest/dev/SSEUsingRESTAPI&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>350</v>
       </c>
@@ -20788,7 +20788,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/troubleshooting.html" target="_blank"&gt;AmazonS3/latest/dev/troubleshooting&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>350</v>
       </c>
@@ -20803,7 +20803,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/troubleshooting.html" target="_blank"&gt;AmazonS3/latest/dev/troubleshooting&lt;/a&gt;&lt;/br&gt;	&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>378</v>
       </c>
@@ -20818,7 +20818,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/serverless-application-model/latest/developerguide/serverless-deploying.html" target="_blank"&gt;serverless-application-model/latest/developerguide/serverless-deploying&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>393</v>
       </c>
@@ -20833,7 +20833,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/APIReference/API_DeleteQueue.html" target="_blank"&gt;AWSSimpleQueueService/latest/APIReference/API_DeleteQueue&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>393</v>
       </c>
@@ -20848,7 +20848,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/APIReference/API_Operations.html" target="_blank"&gt;AWSSimpleQueueService/latest/APIReference/API_Operations&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>393</v>
       </c>
@@ -20863,7 +20863,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/APIReference/API_SetQueueAttributes.html" target="_blank"&gt;AWSSimpleQueueService/latest/APIReference/API_SetQueueAttributes&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>393</v>
       </c>
@@ -20878,7 +20878,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/FIFO-queues.html#FIFO-queues-understanding-logic" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/FIFO-queues.html#FIFO-queues-understanding-logic&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>393</v>
       </c>
@@ -20893,7 +20893,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-create-queue.html" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-create-queue&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>393</v>
       </c>
@@ -20908,7 +20908,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-long-polling.html#sqs-short-long-polling-differences" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-long-polling.html#sqs-short-long-polling-differences&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>393</v>
       </c>
@@ -20923,7 +20923,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-message-lifecycle.html" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-message-lifecycle&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>393</v>
       </c>
@@ -20938,7 +20938,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-visibility-timeout.html#sqs-inflight-messages" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-visibility-timeout.html#sqs-inflight-messages&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>393</v>
       </c>
@@ -20953,7 +20953,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/standard-queues.html#standard-queues-message-order" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/standard-queues.html#standard-queues-message-order&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>393</v>
       </c>
@@ -20968,7 +20968,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/Welcome.html" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/Welcome&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>393</v>
       </c>
@@ -20983,7 +20983,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sqs/faqs/" target="_blank"&gt;sqs/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>393</v>
       </c>
@@ -20998,7 +20998,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/sqs/faqs/ " target="_blank"&gt;sqs/faqs/ &lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>393</v>
       </c>
@@ -21013,7 +21013,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/sqs/faqs/" target="_blank"&gt;sqs/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>393</v>
       </c>
@@ -21028,7 +21028,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSSimpleQueueService/2009-02-01/SQSDeveloperGuide/index.html?IntroductionArticle.html" target="_blank"&gt;AWSSimpleQueueService/2009-02-01/SQSDeveloperGuide/index.html?IntroductionArticle&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>393</v>
       </c>
@@ -21043,7 +21043,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-delay-queues.html" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-delay-queues&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>393</v>
       </c>
@@ -21058,7 +21058,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-long-polling.html" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-long-polling&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>393</v>
       </c>
@@ -21073,7 +21073,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-message-attributes.html" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-message-attributes&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>393</v>
       </c>
@@ -21088,7 +21088,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-visibility-timeout.html" target="_blank"&gt;AWSSimpleQueueService/latest/SQSDeveloperGuide/sqs-visibility-timeout&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>342</v>
       </c>
@@ -21103,7 +21103,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/api/API_CreatePlatformEndpoint.html" target="_blank"&gt;sns/latest/api/API_CreatePlatformEndpoint&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>342</v>
       </c>
@@ -21118,7 +21118,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/json-formats.htm" target="_blank"&gt;sns/latest/dg/json-formats.htm&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>342</v>
       </c>
@@ -21133,7 +21133,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/json-formats.html" target="_blank"&gt;sns/latest/dg/json-formats&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>342</v>
       </c>
@@ -21148,7 +21148,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-custommessage.html" target="_blank"&gt;sns/latest/dg/mobile-push-send-custommessage&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="296" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>342</v>
       </c>
@@ -21163,7 +21163,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-devicetoken.html" target="_blank"&gt;sns/latest/dg/mobile-push-send-devicetoken&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>342</v>
       </c>
@@ -21178,7 +21178,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-register.html" target="_blank"&gt;sns/latest/dg/mobile-push-send-register&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>342</v>
       </c>
@@ -21193,7 +21193,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/SendMessageToHttp.html" target="_blank"&gt;sns/latest/dg/SendMessageToHttp&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>342</v>
       </c>
@@ -21208,7 +21208,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/SNSMessageAttributes.html" target="_blank"&gt;sns/latest/dg/SNSMessageAttributes&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="300" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>342</v>
       </c>
@@ -21223,7 +21223,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/sns/latest/gsg/CreateTopic.html" target="_blank"&gt;sns/latest/gsg/CreateTopic&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>342</v>
       </c>
@@ -21238,7 +21238,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/sns/faqs/" target="_blank"&gt;sns/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>342</v>
       </c>
@@ -21253,7 +21253,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/sns/latest/api/API_Publish.html" target="_blank"&gt;sns/latest/api/API_Publish&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>342</v>
       </c>
@@ -21268,7 +21268,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/sns/latest/dg/message-filtering.html" target="_blank"&gt;sns/latest/dg/message-filtering&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>342</v>
       </c>
@@ -21283,7 +21283,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-devicetoken.html" target="_blank"&gt;sns/latest/dg/mobile-push-send-devicetoken&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>374</v>
       </c>
@@ -21298,7 +21298,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/streams/latest/dev/amazon-kinesis-streams.html" target="_blank"&gt;streams/latest/dev/amazon-kinesis-streams&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="306" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>374</v>
       </c>
@@ -21313,7 +21313,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/streams/latest/dev/what-is-sse.html" target="_blank"&gt;streams/latest/dev/what-is-sse&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="307" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>395</v>
       </c>
@@ -21328,7 +21328,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/STS/latest/APIReference/Welcome.html" target="_blank"&gt;STS/latest/APIReference/Welcome&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;3&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>358</v>
       </c>
@@ -21343,7 +21343,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/amazonswf/latest/developerguide/swf-dg-develop-activity.html" target="_blank"&gt;amazonswf/latest/developerguide/swf-dg-develop-activity&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="309" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>358</v>
       </c>
@@ -21358,7 +21358,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/swf/faqs/" target="_blank"&gt;swf/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;6&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>356</v>
       </c>
@@ -21373,7 +21373,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonVPC/latest/UserGuide/VPC_Route_Tables.html" target="_blank"&gt;AmazonVPC/latest/UserGuide/VPC_Route_Tables&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="311" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>356</v>
       </c>
@@ -21388,7 +21388,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="http://docs.aws.amazon.com/AmazonVPC/latest/UserGuide/vpc-endpoints.html" target="_blank"&gt;AmazonVPC/latest/UserGuide/vpc-endpoints&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>356</v>
       </c>
@@ -21403,7 +21403,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://aws.amazon.com/vpc/faqs/" target="_blank"&gt;vpc/faqs/&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>362</v>
       </c>
@@ -21418,7 +21418,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://d0.awsstatic.com/whitepapers/aws-security-whitepaper.pdf" target="_blank"&gt;whitepapers/aws-security-whitepaper.pdf&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>362</v>
       </c>
@@ -21433,7 +21433,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://d0.awsstatic.com/whitepapers/Security/AWS%20Security%20Whitepaper.pdf" target="_blank"&gt;whitepapers/Security/AWS%20Security%20Whitepaper.pdf&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="315" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>362</v>
       </c>
@@ -21448,7 +21448,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://d0.awsstatic.com/whitepapers/Storage/AWS%20Storage%20Services%20Whitepaper-v9.pdf" target="_blank"&gt;whitepapers/Storage/AWS%20Storage%20Services%20Whitepaper-v9.pdf&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>376</v>
       </c>
@@ -21463,7 +21463,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href="https://docs.aws.amazon.com/xray/latest/devguide/aws-xray.html" target="_blank"&gt;xray/latest/devguide/aws-xray&lt;/a&gt;&lt;/br&gt;&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>376</v>
       </c>

</xml_diff>